<commit_message>
Updated calibrated spdts levels.
</commit_message>
<xml_diff>
--- a/Decoder.xlsx
+++ b/Decoder.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\LFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7667F6D1-23F2-47FD-A31E-59C975C8AD1C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB9F530-E720-492B-ABA7-DFC4E154C5C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31650" yWindow="4545" windowWidth="28800" windowHeight="15435" xr2:uid="{680AAE41-F98C-4C93-B345-C82768ABB2DB}"/>
+    <workbookView xWindow="1545" yWindow="2550" windowWidth="28800" windowHeight="15435" xr2:uid="{680AAE41-F98C-4C93-B345-C82768ABB2DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Voltage</t>
   </si>
@@ -37,6 +43,12 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>Divider</t>
+  </si>
+  <si>
+    <t>LFO</t>
   </si>
 </sst>
 </file>
@@ -81,16 +93,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,15 +414,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321C8C12-E6F5-4826-B808-85B5499B80EA}">
-  <dimension ref="D7:G16"/>
+  <dimension ref="D4:L16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,11 +440,23 @@
       <c r="F7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <v>1.1652916439279599</v>
       </c>
@@ -442,8 +471,22 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <v>1.163</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" ref="J8:J15" si="0">1023*I8/I$16</f>
+        <v>238.76158940397355</v>
+      </c>
+      <c r="K8" s="3">
+        <f>(J8)/2</f>
+        <v>119.38079470198677</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <v>1.57686226129867</v>
       </c>
@@ -452,122 +495,227 @@
         <v>322.62601866170792</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ref="F9:F15" si="0">(E9+E8)/2</f>
+        <f t="shared" ref="F9:F15" si="1">(E9+E8)/2</f>
         <v>280.52234450468427</v>
       </c>
       <c r="G9">
         <f>G8+1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <v>1.5740000000000001</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="0"/>
+        <v>323.13907284768214</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" ref="K9:K15" si="2">(J9+J8)/2</f>
+        <v>280.95033112582786</v>
+      </c>
+      <c r="L9">
+        <f>L8+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <v>1.9922723979715</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" ref="E10:E16" si="1">1023*D10/5</f>
+        <f t="shared" ref="E10:E16" si="3">1023*D10/5</f>
         <v>407.61893262496892</v>
       </c>
       <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>365.12247564333842</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10:G16" si="4">G9+1</f>
+        <v>2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.988</v>
+      </c>
+      <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>365.12247564333842</v>
-      </c>
-      <c r="G10">
-        <f t="shared" ref="G10:G16" si="2">G9+1</f>
+        <v>408.13245033112582</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="2"/>
+        <v>365.63576158940396</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L16" si="5">L9+1</f>
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <v>2.4921276981103202</v>
       </c>
       <c r="E11" s="3">
+        <f t="shared" si="3"/>
+        <v>509.8893270333715</v>
+      </c>
+      <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>509.8893270333715</v>
-      </c>
-      <c r="F11" s="3">
+        <v>458.75412982917021</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="I11" s="2">
+        <v>2.4809999999999999</v>
+      </c>
+      <c r="J11" s="3">
         <f t="shared" si="0"/>
-        <v>458.75412982917021</v>
-      </c>
-      <c r="G11">
+        <v>509.34437086092714</v>
+      </c>
+      <c r="K11" s="3">
         <f t="shared" si="2"/>
+        <v>458.73841059602648</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <v>2.9729729729729701</v>
       </c>
       <c r="E12" s="3">
+        <f t="shared" si="3"/>
+        <v>608.27027027026975</v>
+      </c>
+      <c r="F12" s="3">
         <f t="shared" si="1"/>
-        <v>608.27027027026975</v>
-      </c>
-      <c r="F12" s="3">
+        <v>559.07979865182062</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2.9649999999999999</v>
+      </c>
+      <c r="J12" s="3">
         <f t="shared" si="0"/>
-        <v>559.07979865182062</v>
-      </c>
-      <c r="G12">
+        <v>608.70860927152319</v>
+      </c>
+      <c r="K12" s="3">
         <f t="shared" si="2"/>
+        <v>559.02649006622516</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <v>3.4672181442978101</v>
       </c>
       <c r="E13" s="3">
+        <f t="shared" si="3"/>
+        <v>709.39283232333196</v>
+      </c>
+      <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>709.39283232333196</v>
-      </c>
-      <c r="F13" s="3">
+        <v>658.83155129680085</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="I13" s="2">
+        <v>3.4580000000000002</v>
+      </c>
+      <c r="J13" s="3">
         <f t="shared" si="0"/>
-        <v>658.83155129680085</v>
-      </c>
-      <c r="G13">
+        <v>709.92052980132462</v>
+      </c>
+      <c r="K13" s="3">
         <f t="shared" si="2"/>
+        <v>659.31456953642396</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <v>3.9285714285714199</v>
       </c>
       <c r="E14" s="3">
+        <f t="shared" si="3"/>
+        <v>803.78571428571252</v>
+      </c>
+      <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>803.78571428571252</v>
-      </c>
-      <c r="F14" s="3">
+        <v>756.58927330452229</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3.9169999999999998</v>
+      </c>
+      <c r="J14" s="3">
         <f t="shared" si="0"/>
-        <v>756.58927330452229</v>
-      </c>
-      <c r="G14">
+        <v>804.15231788079473</v>
+      </c>
+      <c r="K14" s="3">
         <f t="shared" si="2"/>
+        <v>757.03642384105967</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <v>4.34264060011827</v>
       </c>
       <c r="E15" s="3">
+        <f t="shared" si="3"/>
+        <v>888.50426678419808</v>
+      </c>
+      <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>888.50426678419808</v>
-      </c>
-      <c r="F15" s="3">
+        <v>846.14499053495524</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="I15" s="2">
+        <v>4.3289999999999997</v>
+      </c>
+      <c r="J15" s="3">
         <f t="shared" si="0"/>
-        <v>846.14499053495524</v>
-      </c>
-      <c r="G15">
+        <v>888.73509933774835</v>
+      </c>
+      <c r="K15" s="3">
         <f t="shared" si="2"/>
+        <v>846.44370860927154</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <v>5</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1023</v>
       </c>
       <c r="F16" s="3">
@@ -575,7 +723,22 @@
         <v>955.75213339209904</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="I16" s="2">
+        <v>4.9829999999999997</v>
+      </c>
+      <c r="J16" s="3">
+        <f>1023*I16/I$16</f>
+        <v>1023</v>
+      </c>
+      <c r="K16" s="3">
+        <f>(J16+J15)/2</f>
+        <v>955.86754966887418</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>

</xml_diff>